<commit_message>
Adjustments to publication notice and code-check
</commit_message>
<xml_diff>
--- a/code-check.xlsx
+++ b/code-check.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Dataset created</t>
   </si>
   <si>
-    <t xml:space="preserve">Replicated?</t>
+    <t xml:space="preserve">Reproduced?</t>
   </si>
   <si>
     <t xml:space="preserve">Figure/Table #</t>
@@ -158,17 +158,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,7 +241,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>